<commit_message>
Aktueller Stand der Dokumentation fuer Release 1.3.5
</commit_message>
<xml_diff>
--- a/00_Allgemein/Aenderungshistorie.xlsx
+++ b/00_Allgemein/Aenderungshistorie.xlsx
@@ -5,21 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\19_Factories\RELEASE\00_Allgemein\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\temp\release_ifs_1.3.5\00_Allgemein\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="7908" tabRatio="575"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="7905" tabRatio="575"/>
   </bookViews>
   <sheets>
-    <sheet name="V1.3.0" sheetId="14" r:id="rId1"/>
-    <sheet name="V1.1.0" sheetId="12" r:id="rId2"/>
-    <sheet name="V1.0" sheetId="11" r:id="rId3"/>
-    <sheet name="Tabelle1" sheetId="10" r:id="rId4"/>
+    <sheet name="V1.3.5" sheetId="15" r:id="rId1"/>
+    <sheet name="V1.3.0" sheetId="14" r:id="rId2"/>
+    <sheet name="V1.1.0" sheetId="12" r:id="rId3"/>
+    <sheet name="V1.0" sheetId="11" r:id="rId4"/>
+    <sheet name="Tabelle1" sheetId="10" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_1Excel_BuiltIn_Print_Titles_1_1">"$#REF!.$#REF!$#REF!:$#REF!$#REF!"</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Tabelle1!$A$1:$B$284</definedName>
+    <definedName name="_FilterDatabase" localSheetId="4" hidden="1">Tabelle1!$A$1:$B$284</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase" localSheetId="0">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_1">"$#REF!.$#REF!$#REF!:$#REF!$#REF!"</definedName>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="398">
   <si>
     <t>Änderung</t>
   </si>
@@ -1190,6 +1192,54 @@
   </si>
   <si>
     <t>Release 1.1</t>
+  </si>
+  <si>
+    <t>Release 1.3.5</t>
+  </si>
+  <si>
+    <t>1.12 (01.03.2017): Querschnittskomponenten dürfen auch von Service Gateways aufgerufen werden (siehe Kapitel 4.2)</t>
+  </si>
+  <si>
+    <t>00_Allgemein\IsyFact-Versionierung.docx</t>
+  </si>
+  <si>
+    <t>0.2 (17.10.2016): Internes Review eingearbeitet
+0.1 (13.10.2016): Initialer Entwurf</t>
+  </si>
+  <si>
+    <t>10_Blaupausen\Integrationsplattform\Grundlagen_interne_Servicekommunikation.docx</t>
+  </si>
+  <si>
+    <t>2.18 (01.03.2017): Anpassung im Kapitel Grundlagen bzgl. Asynchrone Kommunikation und Zugriff auf Querschnittssysteme</t>
+  </si>
+  <si>
+    <t>10_Blaupausen\technische_Architektur\Detailkonzept_Komponente_Service.docx</t>
+  </si>
+  <si>
+    <t>20_Bausteine\Fehlerbehandlung\Konzept_Fehlerbehandlung.docx</t>
+  </si>
+  <si>
+    <t>2.16 (23.01.2017): Vorlageanwendung eingepflegt</t>
+  </si>
+  <si>
+    <t>3.11 (25.01.2017): Vorlageanwendung eingepflegt</t>
+  </si>
+  <si>
+    <t>2.17 (19.12.2016): Vorlageanwendung eingepflegt
+2.16 (10.10.2016): Erweiterung um schemaübergreifende Operationen. Kapitel 10.5</t>
+  </si>
+  <si>
+    <t>1.12 (01.03.2017): Anpassung im Kapitel Realisierung bzgl. Java-Version der Schnittstelle</t>
+  </si>
+  <si>
+    <t>2.26 (20.01.2017): Vorlageanwendung IsyFact eingepflegt
+2.25 (13.12.2016): Beschreibung des Ressourcen Cachings</t>
+  </si>
+  <si>
+    <t>2.14 (31.01.2017): Vorlageanwendung ungepflegt</t>
+  </si>
+  <si>
+    <t>1.12 (26.10.2016): Regeln zur Logerstellung ergänzt.</t>
   </si>
 </sst>
 </file>
@@ -1447,6 +1497,55 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
+          <a:ext cx="1707962" cy="770965"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>222062</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>770965</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
           <a:ext cx="1753682" cy="770965"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1459,7 +1558,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1508,7 +1607,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1908,37 +2007,37 @@
   <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="77.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="156.88671875" style="2" customWidth="1"/>
-    <col min="4" max="256" width="9.109375" style="3" customWidth="1"/>
-    <col min="257" max="16384" width="11.44140625" style="3"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="77.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="156.85546875" style="2" customWidth="1"/>
+    <col min="4" max="256" width="9.140625" style="3" customWidth="1"/>
+    <col min="257" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="15"/>
     </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>313</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="14" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="14" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
@@ -1949,87 +2048,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>357</v>
-      </c>
-      <c r="C6" s="35" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>359</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>361</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>369</v>
+        <v>389</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="35" t="s">
         <v>15</v>
       </c>
@@ -2037,21 +2136,21 @@
         <v>371</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>373</v>
+        <v>390</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="24" customFormat="1" ht="118.8" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
         <v>15</v>
       </c>
@@ -2059,289 +2158,277 @@
         <v>375</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="35" t="s">
-        <v>377</v>
-      </c>
-      <c r="C16" s="36" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="35" t="s">
-        <v>379</v>
-      </c>
-      <c r="C17" s="36" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
+    </row>
+    <row r="17" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="36"/>
+    </row>
+    <row r="18" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
     </row>
@@ -2353,40 +2440,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="77.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="156.88671875" style="2" customWidth="1"/>
-    <col min="4" max="256" width="9.109375" style="3" customWidth="1"/>
-    <col min="257" max="16384" width="11.44140625" style="3"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="77.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="156.85546875" style="2" customWidth="1"/>
+    <col min="4" max="256" width="9.140625" style="3" customWidth="1"/>
+    <col min="257" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="15"/>
     </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>313</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="14" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="14" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
@@ -2397,525 +2484,401 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>316</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>317</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>318</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>319</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>320</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>321</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="29"/>
-    </row>
-    <row r="15" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>322</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>323</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>324</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>325</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>326</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" t="s">
-        <v>327</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="11"/>
-    </row>
-    <row r="22" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>328</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" t="s">
-        <v>329</v>
-      </c>
-      <c r="C23" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" t="s">
-        <v>330</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" t="s">
-        <v>331</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" t="s">
-        <v>332</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" t="s">
-        <v>333</v>
-      </c>
-      <c r="C29" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" t="s">
-        <v>334</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" t="s">
-        <v>335</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" t="s">
-        <v>355</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="11"/>
-    </row>
-    <row r="34" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" t="s">
-        <v>336</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" t="s">
-        <v>337</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" t="s">
-        <v>338</v>
-      </c>
-      <c r="C36" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" t="s">
-        <v>339</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" t="s">
-        <v>340</v>
-      </c>
-      <c r="C38" s="26" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" t="s">
-        <v>341</v>
-      </c>
-      <c r="C39" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" t="s">
-        <v>342</v>
-      </c>
-      <c r="C40" s="29" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="24" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A42" s="32"/>
-      <c r="B42" s="33" t="s">
-        <v>353</v>
-      </c>
-      <c r="C42" s="34"/>
-    </row>
-    <row r="44" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="31" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" s="31" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A46" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B46" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C46" s="26" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A47" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47" s="30" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" s="31" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="31" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B50" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B51" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="31" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B52" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52" s="31" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" s="31" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" s="24" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A54" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" s="26" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B55" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C55" s="26" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B56" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C56" s="30" t="s">
-        <v>349</v>
-      </c>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>357</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>359</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>361</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>363</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>365</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>367</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>369</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>371</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>373</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="24" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>375</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>377</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>379</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2925,32 +2888,604 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C56"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="77.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="156.85546875" style="2" customWidth="1"/>
+    <col min="4" max="256" width="9.140625" style="3" customWidth="1"/>
+    <col min="257" max="16384" width="11.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="15"/>
+    </row>
+    <row r="2" spans="1:3" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="14" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>316</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>317</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>319</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>320</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>321</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="21"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="29"/>
+    </row>
+    <row r="15" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>322</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>323</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>324</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>325</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>326</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>327</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="21"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>328</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>329</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>330</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>331</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>332</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>333</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>334</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s">
+        <v>335</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>355</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="21"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="11"/>
+    </row>
+    <row r="34" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>336</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>337</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>338</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>339</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>340</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" t="s">
+        <v>341</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>342</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="24" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A42" s="32"/>
+      <c r="B42" s="33" t="s">
+        <v>353</v>
+      </c>
+      <c r="C42" s="34"/>
+    </row>
+    <row r="44" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="31" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A46" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="26" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A47" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="31" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="31" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="31" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="31" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="24" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A54" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="26" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>349</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="77.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="156.88671875" style="2" customWidth="1"/>
-    <col min="4" max="256" width="9.109375" style="3" customWidth="1"/>
-    <col min="257" max="16384" width="11.44140625" style="3"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="77.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="156.85546875" style="2" customWidth="1"/>
+    <col min="4" max="256" width="9.140625" style="3" customWidth="1"/>
+    <col min="257" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="15"/>
     </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>313</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>314</v>
       </c>
@@ -2958,7 +3493,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="14" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="14" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
@@ -2969,10 +3504,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="5.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
@@ -2983,7 +3518,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>15</v>
       </c>
@@ -2994,7 +3529,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>15</v>
       </c>
@@ -3005,7 +3540,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>15</v>
       </c>
@@ -3016,7 +3551,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>15</v>
       </c>
@@ -3027,7 +3562,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>15</v>
       </c>
@@ -3038,7 +3573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>15</v>
       </c>
@@ -3049,12 +3584,12 @@
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="21"/>
       <c r="B13" s="25"/>
       <c r="C13" s="29"/>
     </row>
-    <row r="14" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>15</v>
       </c>
@@ -3065,7 +3600,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>15</v>
       </c>
@@ -3076,7 +3611,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
         <v>15</v>
       </c>
@@ -3087,7 +3622,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>15</v>
       </c>
@@ -3098,7 +3633,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>15</v>
       </c>
@@ -3109,7 +3644,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
         <v>15</v>
       </c>
@@ -3120,12 +3655,12 @@
         <v>312</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="21"/>
       <c r="B20" s="22"/>
       <c r="C20" s="11"/>
     </row>
-    <row r="21" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="s">
         <v>15</v>
       </c>
@@ -3136,7 +3671,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="21" t="s">
         <v>15</v>
       </c>
@@ -3147,7 +3682,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
         <v>15</v>
       </c>
@@ -3158,7 +3693,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
         <v>15</v>
       </c>
@@ -3169,7 +3704,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="s">
         <v>15</v>
       </c>
@@ -3180,7 +3715,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
         <v>15</v>
       </c>
@@ -3191,7 +3726,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
         <v>15</v>
       </c>
@@ -3202,7 +3737,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="s">
         <v>15</v>
       </c>
@@ -3213,7 +3748,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
         <v>15</v>
       </c>
@@ -3224,12 +3759,12 @@
         <v>312</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="21"/>
       <c r="B30" s="22"/>
       <c r="C30" s="11"/>
     </row>
-    <row r="31" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="s">
         <v>15</v>
       </c>
@@ -3240,7 +3775,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="s">
         <v>14</v>
       </c>
@@ -3251,7 +3786,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="s">
         <v>14</v>
       </c>
@@ -3262,7 +3797,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="s">
         <v>14</v>
       </c>
@@ -3273,7 +3808,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>14</v>
       </c>
@@ -3284,7 +3819,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>15</v>
       </c>
@@ -3295,7 +3830,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
         <v>14</v>
       </c>
@@ -3313,21 +3848,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:B284"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B236" sqref="B236:B283"/>
+      <selection activeCell="B293" sqref="B293"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="97.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="97.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>309</v>
       </c>
@@ -3335,177 +3870,177 @@
         <v>310</v>
       </c>
     </row>
-    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>311</v>
       </c>
@@ -3513,7 +4048,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>311</v>
       </c>
@@ -3521,7 +4056,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>311</v>
       </c>
@@ -3529,7 +4064,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>311</v>
       </c>
@@ -3537,7 +4072,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>311</v>
       </c>
@@ -3545,7 +4080,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>311</v>
       </c>
@@ -3553,127 +4088,127 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="63" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>311</v>
       </c>
@@ -3681,112 +4216,112 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>311</v>
       </c>
@@ -3794,7 +4329,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>311</v>
       </c>
@@ -3802,7 +4337,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>311</v>
       </c>
@@ -3810,7 +4345,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>311</v>
       </c>
@@ -3818,7 +4353,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>311</v>
       </c>
@@ -3826,127 +4361,127 @@
         <v>117</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="97" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="98" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="99" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="100" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="101" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="102" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="103" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="104" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="105" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="106" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="107" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="108" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="109" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="110" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="111" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="112" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>311</v>
       </c>
@@ -3954,72 +4489,72 @@
         <v>142</v>
       </c>
     </row>
-    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>311</v>
       </c>
@@ -4027,72 +4562,72 @@
         <v>156</v>
       </c>
     </row>
-    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>311</v>
       </c>
@@ -4100,72 +4635,72 @@
         <v>170</v>
       </c>
     </row>
-    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>311</v>
       </c>
@@ -4173,72 +4708,72 @@
         <v>184</v>
       </c>
     </row>
-    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>311</v>
       </c>
@@ -4246,92 +4781,92 @@
         <v>198</v>
       </c>
     </row>
-    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>311</v>
       </c>
@@ -4339,7 +4874,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>311</v>
       </c>
@@ -4347,7 +4882,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>311</v>
       </c>
@@ -4355,72 +4890,72 @@
         <v>218</v>
       </c>
     </row>
-    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B201" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B202" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B203" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B204" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B205" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B206" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>311</v>
       </c>
@@ -4428,147 +4963,147 @@
         <v>232</v>
       </c>
     </row>
-    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B208" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="209" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B209" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="210" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B210" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="211" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B211" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="212" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B212" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="213" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B213" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="214" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B214" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="215" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B215" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="216" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B216" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="217" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B217" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="218" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B218" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="219" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B219" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="220" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B220" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="221" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B221" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="222" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B222" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="223" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B223" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="224" spans="2:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B224" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B225" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B226" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B227" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B228" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B229" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B230" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B231" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B232" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B233" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B234" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B235" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>311</v>
       </c>
@@ -4576,7 +5111,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>311</v>
       </c>
@@ -4584,7 +5119,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>311</v>
       </c>
@@ -4592,72 +5127,72 @@
         <v>263</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B239" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B240" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B241" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B242" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B243" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B244" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B245" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B246" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B247" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B248" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B249" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B250" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B251" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>311</v>
       </c>
@@ -4665,82 +5200,82 @@
         <v>277</v>
       </c>
     </row>
-    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B253" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B254" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B255" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B256" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="257" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B257" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B258" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B259" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B260" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B261" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B262" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B263" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B264" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B265" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B266" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B267" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>311</v>
       </c>
@@ -4748,7 +5283,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>311</v>
       </c>
@@ -4756,72 +5291,72 @@
         <v>294</v>
       </c>
     </row>
-    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B270" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B271" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B272" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B273" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B274" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B275" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B276" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B277" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B278" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B279" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B280" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B281" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="B282" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>311</v>
       </c>
@@ -4829,7 +5364,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <autoFilter ref="A1:B284">
     <filterColumn colId="0">

</xml_diff>